<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758106968695_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758106968695_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758106968695_backup@backdoor.com.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7247C57C-4C8B-4452-9B2F-1B35AD2B08F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -270,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -642,16 +643,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -691,7 +696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -711,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -731,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -751,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -771,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -791,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -811,7 +816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -831,7 +836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -851,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -871,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -891,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -911,7 +916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -931,7 +936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -951,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -971,7 +976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -991,7 +996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1071,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1091,7 +1096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1111,7 +1116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1131,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1171,7 +1176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1191,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1211,7 +1216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1251,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1271,7 +1276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1291,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1311,7 +1316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1351,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1371,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1391,7 +1396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1431,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1451,7 +1456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1471,7 +1476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1491,7 +1496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1511,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1531,7 +1536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1551,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1571,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1591,7 +1596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1611,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1651,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1671,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1711,7 +1716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1731,7 +1736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1751,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1771,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1791,7 +1796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1831,7 +1836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1851,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1871,7 +1876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -1911,7 +1916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -1951,7 +1956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -1971,7 +1976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -1991,7 +1996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2011,7 +2016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2031,7 +2036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2051,7 +2056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2071,7 +2076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2091,7 +2096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>

</xml_diff>